<commit_message>
new changes for jvm
</commit_message>
<xml_diff>
--- a/tony-checksheet.xlsx
+++ b/tony-checksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lei.du/tony-workspace/duleitony-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C4864F-256B-B245-9EC6-C707F6D99335}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61248108-56D7-C742-A911-368017E6808D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="28000" windowHeight="17540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="28000" windowHeight="17540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jvm-memory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="356">
   <si>
     <t>存储内容</t>
   </si>
@@ -914,10 +914,6 @@
 G-CAT</t>
   </si>
   <si>
-    <t>SGT
-JET-S</t>
-  </si>
-  <si>
     <t>■Authorization</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1185,9 +1181,6 @@
 G-CAN</t>
   </si>
   <si>
-    <t>JET-S</t>
-  </si>
-  <si>
     <t>C-REX</t>
   </si>
   <si>
@@ -1200,6 +1193,9 @@
     <t>CAFIS</t>
   </si>
   <si>
+    <t>CARDNET</t>
+  </si>
+  <si>
     <t>JCN</t>
   </si>
   <si>
@@ -1237,6 +1233,9 @@
   </si>
   <si>
     <t>情報処理センター</t>
+  </si>
+  <si>
+    <t>JCN JET-S</t>
   </si>
 </sst>
 </file>
@@ -7590,7 +7589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E1FA1B-4CD5-374F-9B3D-692D90889D71}">
   <dimension ref="B2:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AC103" sqref="AC103"/>
     </sheetView>
   </sheetViews>
@@ -8624,17 +8623,17 @@
   <sheetData>
     <row r="2" spans="2:24" ht="12" customHeight="1">
       <c r="B2" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="2:24" ht="12" customHeight="1">
       <c r="B4" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>
       <c r="G4" s="76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H4" s="76"/>
       <c r="I4" s="76"/>
@@ -8643,20 +8642,20 @@
       <c r="L4" s="76"/>
       <c r="M4" s="31"/>
       <c r="P4" s="76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q4" s="76"/>
       <c r="T4" s="76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U4" s="76"/>
       <c r="X4" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="2:24" ht="12" customHeight="1">
       <c r="G5" s="77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H5" s="77"/>
       <c r="I5" s="77"/>
@@ -8668,32 +8667,32 @@
     </row>
     <row r="7" spans="2:24" ht="12" customHeight="1">
       <c r="B7" s="51" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="53" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="G7" s="54" t="s">
         <v>283</v>
-      </c>
-      <c r="G7" s="54" t="s">
-        <v>284</v>
       </c>
       <c r="H7" s="54"/>
       <c r="K7" s="54" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L7" s="54"/>
       <c r="M7" s="31"/>
       <c r="P7" s="88" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q7" s="89"/>
       <c r="T7" s="53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U7" s="53"/>
       <c r="V7" s="34"/>
       <c r="W7" s="34"/>
       <c r="X7" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="2:24" ht="12" customHeight="1">
@@ -8732,7 +8731,7 @@
       <c r="B10" s="52"/>
       <c r="D10" s="53"/>
       <c r="G10" s="55" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H10" s="56"/>
       <c r="K10" s="54"/>
@@ -8756,13 +8755,13 @@
       <c r="P11" s="90"/>
       <c r="Q11" s="91"/>
       <c r="T11" s="54" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="U11" s="54"/>
       <c r="V11" s="34"/>
       <c r="W11" s="34"/>
       <c r="X11" s="72" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="12" customHeight="1">
@@ -8787,7 +8786,7 @@
       <c r="G13" s="57"/>
       <c r="H13" s="58"/>
       <c r="K13" s="53" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L13" s="53"/>
       <c r="M13" s="31"/>
@@ -8831,14 +8830,14 @@
       <c r="V15" s="34"/>
       <c r="W15" s="34"/>
       <c r="X15" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="2:24" ht="12" customHeight="1">
       <c r="B16" s="52"/>
       <c r="D16" s="53"/>
       <c r="G16" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H16" s="71"/>
       <c r="K16" s="53"/>
@@ -8888,20 +8887,20 @@
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="75" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:24" ht="12" customHeight="1">
       <c r="B19" s="52"/>
       <c r="D19" s="53" t="s">
+        <v>293</v>
+      </c>
+      <c r="G19" s="54" t="s">
         <v>294</v>
-      </c>
-      <c r="G19" s="54" t="s">
-        <v>295</v>
       </c>
       <c r="H19" s="54"/>
       <c r="K19" s="54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L19" s="54"/>
       <c r="M19" s="31"/>
@@ -8944,19 +8943,19 @@
       <c r="R21" s="34"/>
       <c r="S21" s="34"/>
       <c r="T21" s="53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="U21" s="53"/>
       <c r="V21" s="34"/>
       <c r="W21" s="34"/>
       <c r="X21" s="72" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="2:24" ht="12" customHeight="1">
       <c r="B22" s="52"/>
       <c r="D22" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G22" s="54"/>
       <c r="H22" s="54"/>
@@ -9022,13 +9021,13 @@
       <c r="R25" s="34"/>
       <c r="S25" s="34"/>
       <c r="T25" s="84" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="U25" s="85"/>
       <c r="V25" s="34"/>
       <c r="W25" s="34"/>
       <c r="X25" s="54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="2:24" ht="12" customHeight="1">
@@ -9049,10 +9048,10 @@
     </row>
     <row r="27" spans="2:24" ht="12" customHeight="1">
       <c r="B27" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="D27" s="54" t="s">
         <v>302</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>303</v>
       </c>
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
@@ -9079,7 +9078,7 @@
       <c r="K28" s="54"/>
       <c r="L28" s="54"/>
       <c r="P28" s="54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q28" s="54"/>
       <c r="R28" s="54"/>
@@ -9096,7 +9095,7 @@
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
       <c r="G29" s="54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H29" s="54"/>
       <c r="K29" s="54"/>
@@ -9133,7 +9132,7 @@
       <c r="L31" s="54"/>
       <c r="M31" s="31"/>
       <c r="P31" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q31" s="62"/>
       <c r="R31" s="34"/>
@@ -9143,13 +9142,13 @@
       <c r="V31" s="34"/>
       <c r="W31" s="34"/>
       <c r="X31" s="67" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="32" spans="2:24" ht="12" customHeight="1">
       <c r="B32" s="51"/>
       <c r="D32" s="54" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
@@ -9201,7 +9200,7 @@
     </row>
     <row r="35" spans="2:24" ht="12" customHeight="1">
       <c r="B35" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P35" s="34"/>
       <c r="Q35" s="34"/>
@@ -9230,17 +9229,17 @@
     </row>
     <row r="38" spans="2:24" ht="12" customHeight="1">
       <c r="B38" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="2:24" ht="12" customHeight="1">
       <c r="B40" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C40" s="76"/>
       <c r="D40" s="76"/>
       <c r="G40" s="76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H40" s="76"/>
       <c r="I40" s="76"/>
@@ -9249,54 +9248,54 @@
       <c r="L40" s="76"/>
       <c r="M40" s="31"/>
       <c r="P40" s="76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q40" s="76"/>
       <c r="T40" s="76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U40" s="76"/>
       <c r="X40" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="2:24" ht="12" customHeight="1">
       <c r="G41" s="77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H41" s="77"/>
       <c r="I41" s="77"/>
     </row>
     <row r="43" spans="2:24" ht="12" customHeight="1">
       <c r="B43" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="D43" s="81" t="s">
         <v>282</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="G43" s="54" t="s">
         <v>283</v>
-      </c>
-      <c r="G43" s="54" t="s">
-        <v>284</v>
       </c>
       <c r="H43" s="54"/>
       <c r="K43" s="54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L43" s="54"/>
       <c r="M43" s="31"/>
       <c r="P43" s="51" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q43" s="51"/>
       <c r="R43" s="34"/>
       <c r="S43" s="34"/>
       <c r="T43" s="53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U43" s="53"/>
       <c r="V43" s="34"/>
       <c r="W43" s="34"/>
       <c r="X43" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="2:24" ht="12" customHeight="1">
@@ -9356,11 +9355,11 @@
       <c r="B47" s="79"/>
       <c r="D47" s="82"/>
       <c r="G47" s="54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H47" s="54"/>
       <c r="K47" s="55" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L47" s="56"/>
       <c r="M47" s="31"/>
@@ -9371,7 +9370,7 @@
       <c r="V47" s="34"/>
       <c r="W47" s="34"/>
       <c r="X47" s="75" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="48" spans="2:24" ht="12" customHeight="1">
@@ -9422,13 +9421,13 @@
       <c r="R50" s="34"/>
       <c r="S50" s="34"/>
       <c r="T50" s="53" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U50" s="53"/>
       <c r="V50" s="34"/>
       <c r="W50" s="34"/>
       <c r="X50" s="75" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="2:24" ht="12" customHeight="1">
@@ -9455,7 +9454,7 @@
       <c r="G52" s="35"/>
       <c r="H52" s="35"/>
       <c r="K52" s="54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L52" s="54"/>
       <c r="M52" s="31"/>
@@ -9472,7 +9471,7 @@
       <c r="B53" s="79"/>
       <c r="D53" s="82"/>
       <c r="G53" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H53" s="71"/>
       <c r="K53" s="54"/>
@@ -9481,13 +9480,13 @@
       <c r="P53" s="51"/>
       <c r="Q53" s="51"/>
       <c r="T53" s="54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U53" s="54"/>
       <c r="V53" s="34"/>
       <c r="W53" s="34"/>
       <c r="X53" s="72" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="2:24" ht="12" customHeight="1">
@@ -9529,14 +9528,14 @@
     <row r="56" spans="2:24" ht="12" customHeight="1">
       <c r="B56" s="79"/>
       <c r="D56" s="53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G56" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H56" s="54"/>
       <c r="K56" s="70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L56" s="70"/>
       <c r="M56" s="31"/>
@@ -9567,7 +9566,7 @@
       <c r="V57" s="34"/>
       <c r="W57" s="34"/>
       <c r="X57" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="2:24" ht="12" customHeight="1">
@@ -9576,7 +9575,7 @@
       <c r="G58" s="54"/>
       <c r="H58" s="54"/>
       <c r="K58" s="54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L58" s="54"/>
       <c r="M58" s="31"/>
@@ -9593,7 +9592,7 @@
     <row r="59" spans="2:24" ht="12" customHeight="1">
       <c r="B59" s="79"/>
       <c r="D59" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G59" s="54"/>
       <c r="H59" s="54"/>
@@ -9622,13 +9621,13 @@
       <c r="R60" s="34"/>
       <c r="S60" s="34"/>
       <c r="T60" s="53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U60" s="53"/>
       <c r="V60" s="34"/>
       <c r="W60" s="34"/>
       <c r="X60" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61" spans="2:24" ht="12" customHeight="1">
@@ -9651,10 +9650,10 @@
     </row>
     <row r="62" spans="2:24" ht="12" customHeight="1">
       <c r="B62" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="D62" s="54" t="s">
         <v>302</v>
-      </c>
-      <c r="D62" s="54" t="s">
-        <v>303</v>
       </c>
       <c r="G62" s="54"/>
       <c r="H62" s="54"/>
@@ -9676,7 +9675,7 @@
       <c r="G63" s="54"/>
       <c r="H63" s="54"/>
       <c r="K63" s="55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L63" s="56"/>
       <c r="M63" s="31"/>
@@ -9689,7 +9688,7 @@
       <c r="V63" s="34"/>
       <c r="W63" s="34"/>
       <c r="X63" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="2:24" ht="12" customHeight="1">
@@ -9712,7 +9711,7 @@
     <row r="65" spans="2:24" ht="12" customHeight="1">
       <c r="B65" s="51"/>
       <c r="D65" s="54" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G65" s="54"/>
       <c r="H65" s="54"/>
@@ -9755,7 +9754,7 @@
       <c r="L67" s="35"/>
       <c r="M67" s="31"/>
       <c r="P67" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q67" s="62"/>
       <c r="R67" s="34"/>
@@ -9765,7 +9764,7 @@
       <c r="V67" s="34"/>
       <c r="W67" s="34"/>
       <c r="X67" s="67" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="2:24" ht="12" customHeight="1">
@@ -9774,7 +9773,7 @@
       <c r="G68" s="35"/>
       <c r="H68" s="35"/>
       <c r="K68" s="70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L68" s="70"/>
       <c r="M68" s="31"/>
@@ -9815,13 +9814,13 @@
     </row>
     <row r="71" spans="2:24" ht="12" customHeight="1">
       <c r="B71" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="G71" s="53" t="s">
         <v>322</v>
-      </c>
-      <c r="D71" s="43" t="s">
-        <v>283</v>
-      </c>
-      <c r="G71" s="53" t="s">
-        <v>323</v>
       </c>
       <c r="H71" s="53"/>
       <c r="P71" s="38"/>
@@ -9833,13 +9832,13 @@
       <c r="V71" s="34"/>
       <c r="W71" s="34"/>
       <c r="X71" s="44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="2:24" ht="12" customHeight="1">
       <c r="B72" s="52"/>
       <c r="D72" s="43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G72" s="53"/>
       <c r="H72" s="53"/>
@@ -9856,12 +9855,12 @@
     <row r="73" spans="2:24" ht="12" customHeight="1">
       <c r="B73" s="52"/>
       <c r="D73" s="43" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G73" s="53"/>
       <c r="H73" s="53"/>
       <c r="P73" s="52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q73" s="52"/>
       <c r="R73" s="34"/>
@@ -9890,42 +9889,42 @@
     </row>
     <row r="78" spans="2:24" ht="12" customHeight="1">
       <c r="B78" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="79" spans="2:24" ht="12" customHeight="1">
       <c r="B79" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="80" spans="2:24" ht="12" customHeight="1">
       <c r="B80" s="29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="12" customHeight="1">
       <c r="B81" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="12" customHeight="1">
       <c r="B82" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="12" customHeight="1">
       <c r="B83" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="12" customHeight="1">
       <c r="B84" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="12" customHeight="1">
       <c r="B85" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -14116,8 +14115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C0D722-3AC6-F241-B47C-06CF31F15319}">
   <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -14126,7 +14125,7 @@
     <col min="2" max="2" width="18" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="27" customWidth="1"/>
     <col min="4" max="4" width="29.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.1640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.1640625" style="27" customWidth="1"/>
     <col min="6" max="6" width="123.5" style="27" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="27"/>
   </cols>
@@ -14136,67 +14135,58 @@
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="2:6" ht="76">
+    </row>
+    <row r="3" spans="2:6" ht="133">
       <c r="B3" s="25" t="s">
         <v>253</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="D3" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="95">
+    <row r="4" spans="2:6" ht="190">
       <c r="B4" s="25" t="s">
         <v>256</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="25" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" ht="38">
       <c r="B5" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="25" t="s">
+        <v>260</v>
+      </c>
       <c r="D5" s="25" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="F5" s="25" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="38">
+    <row r="6" spans="2:6" ht="57">
       <c r="B6" s="25" t="s">
         <v>267</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="D6" s="25" t="s">
+        <v>267</v>
+      </c>
       <c r="E6" s="25" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="25" t="s">
         <v>268</v>
       </c>
     </row>
@@ -14204,14 +14194,13 @@
       <c r="B7" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="25" t="s">
+        <v>263</v>
+      </c>
       <c r="D7" s="25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="F7" s="25" t="s">
         <v>272</v>
       </c>
     </row>
@@ -14219,30 +14208,29 @@
       <c r="B8" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="25" t="s">
+        <v>265</v>
+      </c>
       <c r="D8" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="E8" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="13" spans="2:6" ht="38">
       <c r="B13" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>354</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>355</v>
-      </c>
       <c r="D13" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="57">
@@ -14253,10 +14241,10 @@
         <v>273</v>
       </c>
       <c r="E14" s="97" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F14" s="97" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -14264,36 +14252,38 @@
         <v>256</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>338</v>
-      </c>
-      <c r="D15" s="25"/>
+        <v>341</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>355</v>
+      </c>
       <c r="E15" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="19" customHeight="1">
       <c r="B16" s="95"/>
       <c r="C16" s="25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="95"/>
       <c r="C17" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
@@ -14301,10 +14291,10 @@
     <row r="18" spans="2:6" ht="57">
       <c r="B18" s="95"/>
       <c r="C18" s="25" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
@@ -14312,27 +14302,27 @@
     <row r="19" spans="2:6">
       <c r="B19" s="95"/>
       <c r="C19" s="25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="96"/>
       <c r="C20" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="2:6">

</xml_diff>